<commit_message>
20190524 fix RIBS Ratio bug.
</commit_message>
<xml_diff>
--- a/Stock Analysis.xlsx
+++ b/Stock Analysis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="142">
   <si>
     <t>日期</t>
   </si>
@@ -293,7 +293,7 @@
     <t>115.77</t>
   </si>
   <si>
-    <t>1466.67%</t>
+    <t>1.06%</t>
   </si>
   <si>
     <t>2019/05/23</t>
@@ -389,10 +389,31 @@
     <t>-85.31 億</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0 %</t>
+    <t>95.22</t>
+  </si>
+  <si>
+    <t>0.37 %</t>
+  </si>
+  <si>
+    <t>8.72</t>
+  </si>
+  <si>
+    <t>0.11 %</t>
+  </si>
+  <si>
+    <t>3.82</t>
+  </si>
+  <si>
+    <t>-10.87</t>
+  </si>
+  <si>
+    <t>-0.82 %</t>
+  </si>
+  <si>
+    <t>31.475</t>
+  </si>
+  <si>
+    <t>-0.03</t>
   </si>
   <si>
     <t>61172</t>
@@ -1182,55 +1203,55 @@
         <v>125</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>125</v>
+        <v>23</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="O6" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="P6" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="Q6" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="R6" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="S6" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="T6" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="U6" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="V6" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="W6" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="X6" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="Y6" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug of OC and USAEx.
</commit_message>
<xml_diff>
--- a/Stock Analysis.xlsx
+++ b/Stock Analysis.xlsx
@@ -353,7 +353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1216,107 +1216,244 @@
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
+          <t>休市</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr">
+        <is>
+          <t>0 %</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>休市</t>
+        </is>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>0 %</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>休市</t>
+        </is>
+      </c>
+      <c r="L7" s="1" t="inlineStr">
+        <is>
+          <t>0 %</t>
+        </is>
+      </c>
+      <c r="M7" s="1" t="inlineStr">
+        <is>
+          <t>休市</t>
+        </is>
+      </c>
+      <c r="N7" s="1" t="inlineStr">
+        <is>
+          <t>0 %</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>31.416</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>-0.013</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>43157</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>-3834</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>1935</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>2923</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>537</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>2896</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>1398</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>12.20 / 10.66</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>107.17</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>0.60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2019/05/28</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>10312.31</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>-21.82</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>-0.21 %</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>1548.68 億</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-56.35 億</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H7" s="1" t="inlineStr">
+      <c r="H8" s="1" t="inlineStr">
         <is>
           <t>0 %</t>
         </is>
       </c>
-      <c r="I7" s="1" t="inlineStr">
+      <c r="I8" s="1" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="J7" s="1" t="inlineStr">
+      <c r="J8" s="1" t="inlineStr">
         <is>
           <t>0 %</t>
         </is>
       </c>
-      <c r="K7" s="1" t="inlineStr">
+      <c r="K8" s="1" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="L7" s="1" t="inlineStr">
+      <c r="L8" s="1" t="inlineStr">
         <is>
           <t>0 %</t>
         </is>
       </c>
-      <c r="M7" s="1" t="inlineStr">
+      <c r="M8" s="1" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="N7" s="1" t="inlineStr">
+      <c r="N8" s="1" t="inlineStr">
         <is>
           <t>0 %</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>43157</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>-3834</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>1935</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>2923</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>537</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>2896</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>1398</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>12.20 / 10.66</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>107.17</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>0.60%</t>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>41796</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>-5195</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>1372</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>2969</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>-204</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>2815</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>1576</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>154</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>11.94 / 10.37</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>106.55</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>1.21%</t>
         </is>
       </c>
     </row>

</xml_diff>